<commit_message>
Commited all 15th May
</commit_message>
<xml_diff>
--- a/Term2/Schedule.xlsx
+++ b/Term2/Schedule.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dks/AMPBA/Term2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92B9A37-496D-004F-B0B6-240F9B7CFBC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AA4368-4052-3345-8051-8B5B94332907}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="560" windowWidth="40040" windowHeight="25100" xr2:uid="{AB14DD4A-F477-E441-9C50-6FB4372967FE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34920" windowHeight="21900" xr2:uid="{AB14DD4A-F477-E441-9C50-6FB4372967FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Term2 schedule" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,7 +147,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-809]dd\-mmm\-yy;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,13 +173,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,11 +202,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
@@ -318,20 +309,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -347,71 +334,71 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -726,120 +713,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12885FAE-96FE-794A-BD4C-8CEFE3CA94C6}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="346" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="273" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="16.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>44304</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="16">
         <v>44318</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="26">
         <v>44321</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>44331</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="3">
         <v>44325</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="26">
         <v>44322</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>44303</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="27">
         <v>44324</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="15">
         <v>44309</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="25">
         <v>44310</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -857,7 +848,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A6" sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,9 +881,9 @@
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -922,10 +913,10 @@
       <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -933,12 +924,12 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -963,12 +954,12 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>